<commit_message>
atualização do tutorialzinho do git
</commit_message>
<xml_diff>
--- a/documentacao/product-backlog-e-outros/Product Backlog Sprint e Requisitos.xlsx
+++ b/documentacao/product-backlog-e-outros/Product Backlog Sprint e Requisitos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\paiotnela\documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Projetos\paiotnela\documentacao\product-backlog-e-outros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1007C042-B0BD-4D88-919B-59057C6F38D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDCEFE9-70C2-4484-95EA-75152074CF8D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -1711,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2089,15 +2089,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="6"/>
-    <col min="3" max="3" width="44" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" style="6" customWidth="1"/>
     <col min="5" max="5" width="15.140625" style="6" customWidth="1"/>
     <col min="6" max="6" width="71.42578125" style="7" customWidth="1"/>
@@ -4505,38 +4505,6 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A152:A154"/>
-    <mergeCell ref="A155:A157"/>
-    <mergeCell ref="A137:A139"/>
-    <mergeCell ref="A140:A142"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="A146:A148"/>
-    <mergeCell ref="A149:A151"/>
-    <mergeCell ref="A127:A129"/>
-    <mergeCell ref="A130:A132"/>
-    <mergeCell ref="A134:A136"/>
-    <mergeCell ref="A118:A120"/>
-    <mergeCell ref="A121:A123"/>
-    <mergeCell ref="A124:A126"/>
-    <mergeCell ref="A108:A110"/>
-    <mergeCell ref="A111:A113"/>
-    <mergeCell ref="A115:A117"/>
-    <mergeCell ref="A98:A101"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="A105:A107"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="A91:A94"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="A85:A87"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A11:A14"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A60:A62"/>
@@ -4553,6 +4521,38 @@
     <mergeCell ref="A72:A74"/>
     <mergeCell ref="A76:A78"/>
     <mergeCell ref="A63:A65"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="A108:A110"/>
+    <mergeCell ref="A111:A113"/>
+    <mergeCell ref="A115:A117"/>
+    <mergeCell ref="A98:A101"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="A105:A107"/>
+    <mergeCell ref="A127:A129"/>
+    <mergeCell ref="A130:A132"/>
+    <mergeCell ref="A134:A136"/>
+    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A121:A123"/>
+    <mergeCell ref="A124:A126"/>
+    <mergeCell ref="A152:A154"/>
+    <mergeCell ref="A155:A157"/>
+    <mergeCell ref="A137:A139"/>
+    <mergeCell ref="A140:A142"/>
+    <mergeCell ref="A143:A145"/>
+    <mergeCell ref="A146:A148"/>
+    <mergeCell ref="A149:A151"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>